<commit_message>
docs: updated product backlog & user stories
</commit_message>
<xml_diff>
--- a/Product Backlog + User Stories.xlsx
+++ b/Product Backlog + User Stories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -38,6 +38,9 @@
     <t>SPRINT #</t>
   </si>
   <si>
+    <t>Done?</t>
+  </si>
+  <si>
     <t>Personalized Travel Recommendations</t>
   </si>
   <si>
@@ -68,7 +71,10 @@
     <t>High</t>
   </si>
   <si>
-    <t>Basic Data / Code Outline + Skeleton</t>
+    <t>Data preprocesing + setting up SQL database</t>
+  </si>
+  <si>
+    <t>-&gt; Last remaining step for part 2 (write code for this on Friday and Monday)</t>
   </si>
   <si>
     <t>User Stories</t>
@@ -141,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -162,9 +168,21 @@
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -355,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -372,69 +390,76 @@
     <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="11" fillId="7" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -705,174 +730,198 @@
       <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="G3" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9">
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10">
         <v>16.0</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="D4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12">
         <v>3.0</v>
       </c>
+      <c r="G4" s="13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="9">
-        <v>12.0</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="E5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="12">
         <v>3.0</v>
       </c>
+      <c r="G5" s="13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="C6" s="10">
         <v>8.0</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="D6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="14">
         <v>2.0</v>
       </c>
+      <c r="G6" s="13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10">
+        <v>14.0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G8" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="9">
-        <v>14.0</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="11">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="E9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="12">
         <v>1.0</v>
       </c>
+      <c r="G9" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="12"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -1899,13 +1948,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>19</v>
+      <c r="A2" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1916,265 +1965,265 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="C3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="E3" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>26</v>
+      <c r="H3" s="20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="18">
+      <c r="A4" s="21">
         <v>1.0</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="D4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="21">
+      <c r="E4" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="24">
         <v>16.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="18">
+      <c r="A5" s="21">
         <v>2.0</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="22" t="s">
+      <c r="B5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="21">
+      <c r="E5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="24">
         <v>12.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="18">
+      <c r="A6" s="21">
         <v>3.0</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="22" t="s">
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="21">
+      <c r="E6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="24">
         <v>6.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="18">
+      <c r="A7" s="21">
         <v>4.0</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="23" t="s">
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="21">
+      <c r="E7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="24">
         <v>14.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="26">
+      <c r="A8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="27"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="26">
+      <c r="A9" s="30"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="27"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26">
+      <c r="A10" s="30"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="27"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26">
+      <c r="A11" s="30"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="27"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26">
+      <c r="A12" s="30"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26">
+      <c r="A13" s="30"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="27"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26">
+      <c r="A14" s="30"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26">
+      <c r="A15" s="30"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="27"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26">
+      <c r="A16" s="30"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26">
+      <c r="A17" s="30"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29">
         <v>0.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32">
+      <c r="A18" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35">
         <f>SUM(H4:H17)</f>
         <v>48</v>
       </c>

</xml_diff>